<commit_message>
adding link to preloader
</commit_message>
<xml_diff>
--- a/questions/aoa_excel.xlsx
+++ b/questions/aoa_excel.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/031fa08f5ca4ffcf/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\farde\OneDrive\Desktop\QPG\Question-Paper-Generator\questions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="15" documentId="8_{A8B72DE0-6B81-47B4-8233-ED5480098206}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{77F77458-F3A6-4F80-AB78-BDF2316D65C8}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F6A0EB3-D3B9-460B-969E-5AAF0ED4BEAF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{FF49C881-8EEE-498F-8C94-782963FB2985}"/>
   </bookViews>
@@ -571,13 +571,14 @@
   <dimension ref="A1:B26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="118.140625" customWidth="1"/>
     <col min="2" max="2" width="55.28515625" customWidth="1"/>
+    <col min="3" max="3" width="27.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>